<commit_message>
DOCS: Updated planning, add log
</commit_message>
<xml_diff>
--- a/Templates/Planning/Verboom_Planning_Project_Freedom_V2.xlsx
+++ b/Templates/Planning/Verboom_Planning_Project_Freedom_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeroe\Documents\Projects\Examen portfolio\Losse Bewijzen die ik vast wel kan gebruiken\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5520172-6FF7-4898-8534-3958613DB51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8DCCFEC-DE9D-469D-BF57-9E85CD206FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12756" xr2:uid="{67E08020-2BB4-44A8-BCC5-26A17469E308}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Planning</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>Eennalaatste dag van sprint</t>
+  </si>
+  <si>
+    <t>Nieuwe user stories maken</t>
+  </si>
+  <si>
+    <t>Eind eerste week sprint</t>
+  </si>
+  <si>
+    <t>4 uur</t>
   </si>
 </sst>
 </file>
@@ -786,10 +795,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1050,6 +1059,23 @@
         <v>45</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>5</v>
@@ -1062,6 +1088,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>